<commit_message>
Lucia's code checking the accuracy
Check the accuracy with Lucia's code and the coreRxnMat is the same, and the accuracy is the same
</commit_message>
<xml_diff>
--- a/Thresholding/StanDep/MatchComparisonResults.xlsx
+++ b/Thresholding/StanDep/MatchComparisonResults.xlsx
@@ -13,7 +13,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>MatchPercentage</t>
+  </si>
   <si>
     <t>MatchPercentage</t>
   </si>
@@ -78,247 +81,247 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>85.044247787610615</v>
+        <v>49.490925188136345</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>85.044247787610615</v>
+        <v>49.490925188136345</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>85.044247787610615</v>
+        <v>49.490925188136345</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>85.044247787610615</v>
+        <v>49.490925188136345</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>85.044247787610615</v>
+        <v>49.490925188136345</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>85.044247787610615</v>
+        <v>49.490925188136345</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>85.044247787610615</v>
+        <v>49.490925188136345</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>85.044247787610615</v>
+        <v>49.490925188136345</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>85.044247787610615</v>
+        <v>49.490925188136345</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>85.044247787610615</v>
+        <v>49.490925188136345</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>85.044247787610615</v>
+        <v>49.490925188136345</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>85.044247787610615</v>
+        <v>49.490925188136345</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>85.044247787610615</v>
+        <v>49.490925188136345</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>85.044247787610615</v>
+        <v>49.490925188136345</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>85.044247787610615</v>
+        <v>49.490925188136345</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>85.044247787610615</v>
+        <v>49.490925188136345</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>85.044247787610615</v>
+        <v>49.490925188136345</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>85.044247787610615</v>
+        <v>49.490925188136345</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>85.044247787610615</v>
+        <v>49.490925188136345</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>85.044247787610615</v>
+        <v>49.490925188136345</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>85.044247787610615</v>
+        <v>49.490925188136345</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>85.044247787610615</v>
+        <v>49.490925188136345</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>85.044247787610615</v>
+        <v>49.490925188136345</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>85.044247787610615</v>
+        <v>49.490925188136345</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>85.044247787610615</v>
+        <v>49.490925188136345</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>85.044247787610615</v>
+        <v>49.490925188136345</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>85.044247787610615</v>
+        <v>49.490925188136345</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>85.044247787610615</v>
+        <v>49.490925188136345</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>85.044247787610615</v>
+        <v>49.490925188136345</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>85.044247787610615</v>
+        <v>49.490925188136345</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>85.044247787610615</v>
+        <v>49.490925188136345</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>85.044247787610615</v>
+        <v>49.490925188136345</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>85.044247787610615</v>
+        <v>49.490925188136345</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>85.044247787610615</v>
+        <v>49.490925188136345</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>85.044247787610615</v>
+        <v>49.490925188136345</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>85.044247787610615</v>
+        <v>49.490925188136345</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>85.044247787610615</v>
+        <v>49.490925188136345</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>85.044247787610615</v>
+        <v>49.490925188136345</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>85.044247787610615</v>
+        <v>49.490925188136345</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0">
-        <v>85.044247787610615</v>
+        <v>49.490925188136345</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>85.044247787610615</v>
+        <v>49.490925188136345</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0">
-        <v>85.044247787610615</v>
+        <v>49.490925188136345</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0">
-        <v>85.044247787610615</v>
+        <v>49.490925188136345</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0">
-        <v>85.044247787610615</v>
+        <v>49.712262062859672</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0">
-        <v>85.044247787610615</v>
+        <v>49.490925188136345</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0">
-        <v>85.044247787610615</v>
+        <v>49.490925188136345</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0">
-        <v>85.044247787610615</v>
+        <v>49.490925188136345</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0">
-        <v>85.044247787610615</v>
+        <v>49.490925188136345</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improve StanDep code and HKG_HKR
</commit_message>
<xml_diff>
--- a/Thresholding/StanDep/MatchComparisonResults.xlsx
+++ b/Thresholding/StanDep/MatchComparisonResults.xlsx
@@ -13,7 +13,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+  <si>
+    <t>HK_R_acc_SD</t>
+  </si>
   <si>
     <t>HK_R_acc_SD</t>
   </si>
@@ -90,247 +93,247 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>98.862251117431938</v>
+        <v>99.360146252285205</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>98.821617228768787</v>
+        <v>99.360146252285205</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>98.821617228768787</v>
+        <v>99.360146252285205</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>98.821617228768787</v>
+        <v>99.360146252285205</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>98.821617228768787</v>
+        <v>99.360146252285205</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>98.821617228768787</v>
+        <v>99.360146252285205</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>98.212108898821612</v>
+        <v>99.268738574040214</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>98.821617228768787</v>
+        <v>99.268738574040214</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>98.740349451442498</v>
+        <v>99.268738574040214</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>98.212108898821612</v>
+        <v>99.268738574040214</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>98.821617228768787</v>
+        <v>99.268738574040214</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>98.740349451442498</v>
+        <v>99.268738574040214</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>98.212108898821612</v>
+        <v>99.268738574040214</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>98.212108898821612</v>
+        <v>99.268738574040214</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>98.212108898821612</v>
+        <v>99.268738574040214</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>98.821617228768787</v>
+        <v>99.268738574040214</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>98.821617228768787</v>
+        <v>99.268738574040214</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>98.740349451442498</v>
+        <v>99.268738574040214</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>98.252742787484763</v>
+        <v>99.634369287020107</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>98.252742787484763</v>
+        <v>99.634369287020107</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>98.252742787484763</v>
+        <v>99.634369287020107</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>98.90288500609509</v>
+        <v>99.360146252285205</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>98.293376676147901</v>
+        <v>99.360146252285205</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>98.293376676147901</v>
+        <v>99.360146252285205</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>98.212108898821612</v>
+        <v>99.314442413162709</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>98.212108898821612</v>
+        <v>99.314442413162709</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>98.293376676147901</v>
+        <v>99.314442413162709</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>98.780983340105649</v>
+        <v>99.268738574040214</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>98.780983340105649</v>
+        <v>99.268738574040214</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>98.780983340105649</v>
+        <v>99.268738574040214</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>98.740349451442498</v>
+        <v>99.405850091407672</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>98.740349451442498</v>
+        <v>99.405850091407672</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>98.740349451442498</v>
+        <v>99.360146252285205</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>98.862251117431938</v>
+        <v>99.360146252285205</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>98.821617228768787</v>
+        <v>99.360146252285205</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>98.293376676147901</v>
+        <v>99.360146252285205</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>98.821617228768787</v>
+        <v>99.360146252285205</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>98.821617228768787</v>
+        <v>99.360146252285205</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>98.90288500609509</v>
+        <v>99.405850091407672</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0">
-        <v>98.212108898821612</v>
+        <v>99.268738574040214</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>98.212108898821612</v>
+        <v>99.268738574040214</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0">
-        <v>98.212108898821612</v>
+        <v>99.268738574040214</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0">
-        <v>98.293376676147901</v>
+        <v>99.314442413162709</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0">
-        <v>98.212108898821612</v>
+        <v>99.268738574040214</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0">
-        <v>98.252742787484763</v>
+        <v>99.268738574040214</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0">
-        <v>98.740349451442498</v>
+        <v>99.268738574040214</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0">
-        <v>98.293376676147901</v>
+        <v>99.268738574040214</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0">
-        <v>98.740349451442498</v>
+        <v>99.268738574040214</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new hk list for the StanDep
</commit_message>
<xml_diff>
--- a/Thresholding/StanDep/MatchComparisonResults.xlsx
+++ b/Thresholding/StanDep/MatchComparisonResults.xlsx
@@ -13,7 +13,22 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+  <si>
+    <t>HK_R_acc_SD</t>
+  </si>
+  <si>
+    <t>HK_R_acc_SD</t>
+  </si>
+  <si>
+    <t>HK_R_acc_SD</t>
+  </si>
+  <si>
+    <t>HK_R_acc_SD</t>
+  </si>
+  <si>
+    <t>HK_R_acc_SD</t>
+  </si>
   <si>
     <t>HK_R_acc_SD</t>
   </si>
@@ -117,7 +132,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2">
@@ -152,62 +167,62 @@
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>99.890109890109898</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>99.890109890109898</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>99.890109890109898</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>99.890109890109898</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>99.890109890109898</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>99.890109890109898</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>99.890109890109898</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>99.890109890109898</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>99.890109890109898</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>99.890109890109898</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>99.890109890109898</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>99.890109890109898</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20">
@@ -242,32 +257,32 @@
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>99.890109890109898</v>
+        <v>100</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>99.890109890109898</v>
+        <v>100</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>99.890109890109898</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>99.890109890109898</v>
+        <v>100</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>99.890109890109898</v>
+        <v>100</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>99.890109890109898</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32">
@@ -317,47 +332,47 @@
     </row>
     <row r="41">
       <c r="A41" s="0">
-        <v>99.890109890109898</v>
+        <v>100</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>99.890109890109898</v>
+        <v>100</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0">
-        <v>99.890109890109898</v>
+        <v>100</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0">
-        <v>99.890109890109898</v>
+        <v>100</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0">
-        <v>99.890109890109898</v>
+        <v>100</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0">
-        <v>99.890109890109898</v>
+        <v>100</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0">
-        <v>99.890109890109898</v>
+        <v>100</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0">
-        <v>99.890109890109898</v>
+        <v>100</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0">
-        <v>99.890109890109898</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>